<commit_message>
Complete rework of the assign.py class
</commit_message>
<xml_diff>
--- a/MatchTA_Server/Capstone_Input_Files/File4-TA Grader Assignment_Spring_25_Final.xlsx
+++ b/MatchTA_Server/Capstone_Input_Files/File4-TA Grader Assignment_Spring_25_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TTU-09-23-23\service\TTU\2024-2025\student support committee\2025springAssignment\TA-grader assignment project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/768b4079c1f233a9/Senior Classes/Working Project/MatchTA_Server/Capstone_Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DD350C1-B03F-41BD-9E0E-2C0E44BDCC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{8DD350C1-B03F-41BD-9E0E-2C0E44BDCC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C09DE2E1-ABA5-40FA-9D76-C8A537BD7DD2}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4110" yWindow="3450" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V1-TAgrader based Assignment " sheetId="6" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="224">
   <si>
     <t xml:space="preserve">Select TA/graders for your course-section </t>
   </si>
@@ -361,9 +361,6 @@
     <t>Room Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Undergradaute courses </t>
-  </si>
-  <si>
     <t>Scott Franklin</t>
   </si>
   <si>
@@ -545,9 +542,6 @@
   </si>
   <si>
     <t>Computer Networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graduate courses </t>
   </si>
   <si>
     <t>Yuanlin Zhang</t>
@@ -764,7 +758,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -802,14 +796,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -980,7 +966,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,18 +987,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1024,7 +998,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1081,21 +1055,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1169,7 +1128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1178,252 +1137,243 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1657,21 +1607,21 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="15.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.86328125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="8" customWidth="1"/>
     <col min="3" max="3" width="10" style="9" customWidth="1"/>
-    <col min="4" max="4" width="45.26953125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="50.26953125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="30.40625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="11.40625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="30.54296875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="11.40625" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="50.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
@@ -1686,7 +1636,7 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:8" ht="62">
+    <row r="2" spans="1:8" ht="63">
       <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
@@ -1704,7 +1654,7 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" ht="16">
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1722,7 +1672,7 @@
       <c r="G3"/>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" ht="16">
+    <row r="4" spans="1:8" ht="15.75">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -1740,7 +1690,7 @@
       <c r="G4"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" ht="16">
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
@@ -1758,7 +1708,7 @@
       <c r="G5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" ht="30.5">
+    <row r="6" spans="1:8" ht="30">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1794,7 +1744,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" ht="32">
+    <row r="8" spans="1:8" ht="31.5">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -1812,7 +1762,7 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" ht="16">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="13" t="s">
         <v>19</v>
       </c>
@@ -1830,7 +1780,7 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" ht="16">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="13" t="s">
         <v>21</v>
       </c>
@@ -1866,7 +1816,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" ht="16">
+    <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
@@ -1884,7 +1834,7 @@
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:8" s="12" customFormat="1" ht="30.5">
+    <row r="13" spans="1:8" s="12" customFormat="1" ht="30">
       <c r="A13" s="13" t="s">
         <v>27</v>
       </c>
@@ -1898,7 +1848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16">
+    <row r="14" spans="1:8" ht="15.75">
       <c r="A14" s="13" t="s">
         <v>29</v>
       </c>
@@ -1916,7 +1866,7 @@
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8" ht="16">
+    <row r="15" spans="1:8" ht="15.75">
       <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
@@ -1934,7 +1884,7 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" ht="16">
+    <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="13" t="s">
         <v>33</v>
       </c>
@@ -1952,7 +1902,7 @@
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" ht="16">
+    <row r="17" spans="1:8" ht="15.75">
       <c r="A17" s="13" t="s">
         <v>35</v>
       </c>
@@ -1970,7 +1920,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" ht="16">
+    <row r="18" spans="1:8" ht="15.75">
       <c r="A18" s="13" t="s">
         <v>37</v>
       </c>
@@ -1988,7 +1938,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="16">
+    <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="13" t="s">
         <v>39</v>
       </c>
@@ -2006,7 +1956,7 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" ht="16">
+    <row r="20" spans="1:8" ht="15.75">
       <c r="A20" s="13" t="s">
         <v>41</v>
       </c>
@@ -2024,7 +1974,7 @@
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" ht="16">
+    <row r="21" spans="1:8" ht="15.75">
       <c r="A21" s="13" t="s">
         <v>43</v>
       </c>
@@ -2042,7 +1992,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" ht="16">
+    <row r="22" spans="1:8" ht="15.75">
       <c r="A22" s="13" t="s">
         <v>45</v>
       </c>
@@ -2060,7 +2010,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:8" ht="16">
+    <row r="23" spans="1:8" ht="15.75">
       <c r="A23" s="13" t="s">
         <v>47</v>
       </c>
@@ -2078,7 +2028,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" ht="16">
+    <row r="24" spans="1:8" ht="30">
       <c r="A24" s="13" t="s">
         <v>49</v>
       </c>
@@ -2096,7 +2046,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" ht="16">
+    <row r="25" spans="1:8" ht="15.75">
       <c r="A25" s="13" t="s">
         <v>51</v>
       </c>
@@ -2114,7 +2064,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" ht="16">
+    <row r="26" spans="1:8" ht="31.5">
       <c r="A26" s="13" t="s">
         <v>53</v>
       </c>
@@ -2132,7 +2082,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" ht="16">
+    <row r="27" spans="1:8" ht="15.75">
       <c r="A27" s="13" t="s">
         <v>56</v>
       </c>
@@ -2150,7 +2100,7 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" ht="16">
+    <row r="28" spans="1:8" ht="31.5">
       <c r="A28" s="13" t="s">
         <v>57</v>
       </c>
@@ -2168,7 +2118,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8" ht="16">
+    <row r="29" spans="1:8" ht="15.75">
       <c r="A29" s="13" t="s">
         <v>59</v>
       </c>
@@ -2186,7 +2136,7 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8" ht="16">
+    <row r="30" spans="1:8" ht="15.75">
       <c r="A30" s="13" t="s">
         <v>61</v>
       </c>
@@ -2204,7 +2154,7 @@
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:8" ht="32">
+    <row r="31" spans="1:8" ht="45">
       <c r="A31" s="13" t="s">
         <v>63</v>
       </c>
@@ -2222,7 +2172,7 @@
       <c r="G31"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="1:8" ht="32">
+    <row r="32" spans="1:8" ht="31.5">
       <c r="A32" s="13" t="s">
         <v>65</v>
       </c>
@@ -2240,7 +2190,7 @@
       <c r="G32"/>
       <c r="H32"/>
     </row>
-    <row r="33" spans="1:8" ht="16">
+    <row r="33" spans="1:8" ht="15.75">
       <c r="A33" s="21" t="s">
         <v>67</v>
       </c>
@@ -2258,7 +2208,7 @@
       <c r="G33"/>
       <c r="H33"/>
     </row>
-    <row r="34" spans="1:8" ht="16">
+    <row r="34" spans="1:8" ht="15.75">
       <c r="A34" s="21" t="s">
         <v>70</v>
       </c>
@@ -2276,7 +2226,7 @@
       <c r="G34"/>
       <c r="H34"/>
     </row>
-    <row r="35" spans="1:8" ht="16">
+    <row r="35" spans="1:8" ht="15.75">
       <c r="A35" s="21" t="s">
         <v>72</v>
       </c>
@@ -2294,12 +2244,12 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
-    <row r="36" spans="1:8" ht="16">
+    <row r="36" spans="1:8" ht="15.75">
       <c r="A36" s="65" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B36" s="66" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C36" s="15">
         <v>20</v>
@@ -2312,7 +2262,7 @@
       <c r="G36"/>
       <c r="H36"/>
     </row>
-    <row r="37" spans="1:8" ht="16">
+    <row r="37" spans="1:8" ht="15.75">
       <c r="A37" s="21" t="s">
         <v>75</v>
       </c>
@@ -2330,7 +2280,7 @@
       <c r="G37"/>
       <c r="H37"/>
     </row>
-    <row r="38" spans="1:8" ht="30.5">
+    <row r="38" spans="1:8" ht="30">
       <c r="A38" s="21" t="s">
         <v>77</v>
       </c>
@@ -2348,7 +2298,7 @@
       <c r="G38"/>
       <c r="H38"/>
     </row>
-    <row r="39" spans="1:8" ht="16">
+    <row r="39" spans="1:8" ht="15.75">
       <c r="A39" s="21" t="s">
         <v>79</v>
       </c>
@@ -2366,7 +2316,7 @@
       <c r="G39"/>
       <c r="H39"/>
     </row>
-    <row r="40" spans="1:8" ht="16">
+    <row r="40" spans="1:8" ht="31.5">
       <c r="A40" s="50" t="s">
         <v>81</v>
       </c>
@@ -2384,7 +2334,7 @@
       <c r="G40"/>
       <c r="H40"/>
     </row>
-    <row r="41" spans="1:8" ht="16">
+    <row r="41" spans="1:8" ht="15.75">
       <c r="A41" s="54" t="s">
         <v>83</v>
       </c>
@@ -2402,7 +2352,7 @@
       <c r="G41"/>
       <c r="H41"/>
     </row>
-    <row r="42" spans="1:8" ht="16">
+    <row r="42" spans="1:8" ht="15.75">
       <c r="A42" s="54"/>
       <c r="B42" s="55"/>
       <c r="C42" s="56"/>
@@ -2437,28 +2387,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0C579A-A634-40CD-9F38-6DE31738D8E0}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="20.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="20.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1328125" style="42" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="42" customWidth="1"/>
-    <col min="4" max="4" width="28.1328125" style="43" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.86328125" style="44" customWidth="1"/>
-    <col min="9" max="9" width="8" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.40625" customWidth="1"/>
+    <col min="1" max="2" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.5">
+    <row r="1" spans="1:10" ht="33">
       <c r="A1" s="81" t="s">
         <v>86</v>
       </c>
@@ -2472,7 +2421,7 @@
       <c r="I1" s="81"/>
       <c r="J1" s="81"/>
     </row>
-    <row r="2" spans="1:10" ht="31">
+    <row r="2" spans="1:10" ht="38.25">
       <c r="A2" s="6" t="s">
         <v>87</v>
       </c>
@@ -2502,157 +2451,172 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="45" customHeight="1">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="10">
+        <v>1412</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
+      <c r="D3" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="59"/>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1">
       <c r="A4" s="10">
-        <v>1412</v>
+        <v>3350</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
-    </row>
-    <row r="5" spans="1:10" ht="61">
+      <c r="G4" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="33">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30">
       <c r="A5" s="10">
         <v>3350</v>
       </c>
       <c r="B5" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>101</v>
-      </c>
       <c r="F5" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I5" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="61">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="10">
-        <v>3350</v>
+        <v>3361</v>
       </c>
       <c r="B6" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>192</v>
+        <v>106</v>
+      </c>
+      <c r="D6" s="82" t="s">
+        <v>191</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I6" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45.75">
+    <row r="7" spans="1:10" ht="30">
       <c r="A7" s="10">
         <v>3361</v>
       </c>
       <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="83"/>
+      <c r="E7" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="33">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15">
+      <c r="A8" s="10">
+        <v>3364</v>
+      </c>
+      <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="84" t="s">
-        <v>193</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="33">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="45.75">
-      <c r="A8" s="10">
-        <v>3361</v>
-      </c>
-      <c r="B8" s="10">
-        <v>2</v>
-      </c>
       <c r="C8" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="85"/>
+        <v>112</v>
+      </c>
+      <c r="D8" s="82" t="s">
+        <v>192</v>
+      </c>
       <c r="E8" s="34" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="I8" s="33">
-        <v>121</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="33.950000000000003" customHeight="1">
@@ -2660,889 +2624,911 @@
         <v>3364</v>
       </c>
       <c r="B9" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="83"/>
+      <c r="E9" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="84" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>114</v>
-      </c>
       <c r="F9" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H9" s="34" t="s">
         <v>116</v>
       </c>
       <c r="I9" s="33">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="20.149999999999999" customHeight="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="10">
-        <v>3364</v>
+        <v>3365</v>
       </c>
       <c r="B10" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="85"/>
+        <v>99</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>193</v>
+      </c>
       <c r="E10" s="34" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G10" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="34" t="s">
-        <v>117</v>
-      </c>
       <c r="I10" s="33">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="45.75">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30">
       <c r="A11" s="10">
         <v>3365</v>
       </c>
       <c r="B11" s="10">
+        <v>2</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="33">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15">
+      <c r="A12" s="10">
+        <v>3368</v>
+      </c>
+      <c r="B12" s="10">
         <v>1</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="28" t="s">
+      <c r="C12" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="E11" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="I11" s="33">
+      <c r="E12" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="33" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="45.75">
-      <c r="A12" s="10">
-        <v>3365</v>
-      </c>
-      <c r="B12" s="10">
-        <v>2</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>99</v>
-      </c>
       <c r="H12" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I12" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30.5">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="10">
-        <v>3368</v>
+        <v>3375</v>
       </c>
       <c r="B13" s="10">
         <v>1</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I13" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30.5">
-      <c r="A14" s="10">
+    <row r="14" spans="1:10" ht="30">
+      <c r="A14" s="24">
         <v>3375</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="24">
+        <v>2</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30">
+      <c r="A15" s="10">
+        <v>3383</v>
+      </c>
+      <c r="B15" s="10">
         <v>1</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="28" t="s">
+      <c r="C15" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E15" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="33">
+      <c r="G15" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45.75">
-      <c r="A15" s="24">
-        <v>3375</v>
-      </c>
-      <c r="B15" s="24">
-        <v>2</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="I15" s="35">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30.5">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="10">
         <v>3383</v>
       </c>
       <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="33">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15">
+      <c r="A17" s="10">
+        <v>4331</v>
+      </c>
+      <c r="B17" s="10">
         <v>1</v>
       </c>
-      <c r="C16" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="I16" s="33">
+      <c r="C17" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30.5">
-      <c r="A17" s="10">
-        <v>3383</v>
-      </c>
-      <c r="B17" s="10">
-        <v>2</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="I17" s="33">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="61">
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="10">
         <v>4331</v>
       </c>
       <c r="B18" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="H18" s="34" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="I18" s="33">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="61">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" s="10">
         <v>4331</v>
       </c>
       <c r="B19" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="I19" s="33">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="61">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="10">
-        <v>4331</v>
+        <v>4352</v>
       </c>
       <c r="B20" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>200</v>
       </c>
       <c r="E20" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="F20" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>143</v>
-      </c>
       <c r="H20" s="34" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="I20" s="33">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="30.5">
-      <c r="A21" s="10">
-        <v>4352</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15">
+      <c r="A21" s="15">
+        <v>4354</v>
       </c>
       <c r="B21" s="10">
         <v>1</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>202</v>
+        <v>146</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>201</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I21" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30.5">
+    <row r="22" spans="1:9" ht="30">
       <c r="A22" s="15">
-        <v>4354</v>
+        <v>4366</v>
       </c>
       <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>203</v>
+        <v>149</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>202</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="I22" s="33">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45.75">
-      <c r="A23" s="15">
-        <v>4366</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15">
+      <c r="A23" s="10">
+        <v>4379</v>
       </c>
       <c r="B23" s="10">
         <v>1</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>204</v>
+        <v>152</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="I23" s="33">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30.5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" s="10">
-        <v>4379</v>
+        <v>4392</v>
       </c>
       <c r="B24" s="10">
         <v>1</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>153</v>
+        <v>203</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="I24" s="33">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15">
+      <c r="A25" s="25">
+        <v>5000</v>
+      </c>
+      <c r="B25" s="25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="37"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.95" customHeight="1">
+      <c r="A26" s="10">
+        <v>5120</v>
+      </c>
+      <c r="B26" s="10">
+        <v>1</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" s="33">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.95" customHeight="1">
+      <c r="A27" s="10">
+        <v>5120</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="80"/>
+      <c r="E27" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="33"/>
+    </row>
+    <row r="28" spans="1:9" ht="30">
+      <c r="A28" s="10">
+        <v>5331</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="33">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15">
+      <c r="A29" s="10">
+        <v>5331</v>
+      </c>
+      <c r="B29" s="10">
+        <v>2</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30.5">
-      <c r="A25" s="10">
-        <v>4392</v>
-      </c>
-      <c r="B25" s="10">
-        <v>1</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G25" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" s="33">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A26" s="86" t="s">
-        <v>157</v>
-      </c>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="86"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A27" s="86"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="86"/>
-    </row>
-    <row r="28" spans="1:10" ht="30.5">
-      <c r="A28" s="25">
-        <v>5000</v>
-      </c>
-      <c r="B28" s="25">
-        <v>1</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="37"/>
-    </row>
-    <row r="29" spans="1:10" ht="30.5">
-      <c r="A29" s="10">
-        <v>5120</v>
-      </c>
-      <c r="B29" s="10">
-        <v>1</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="79" t="s">
-        <v>206</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="I29" s="33">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="30.5">
+    <row r="30" spans="1:9" ht="30">
       <c r="A30" s="10">
-        <v>5120</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>164</v>
+        <v>5331</v>
+      </c>
+      <c r="B30" s="10">
+        <v>3</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30" s="80"/>
+        <v>122</v>
+      </c>
+      <c r="D30" s="67" t="s">
+        <v>223</v>
+      </c>
       <c r="E30" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="33"/>
-    </row>
-    <row r="31" spans="1:10" ht="61">
+        <v>165</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" s="33">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30">
       <c r="A31" s="10">
         <v>5331</v>
       </c>
       <c r="B31" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>207</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="I31" s="33">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="27" customHeight="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="27" customHeight="1">
       <c r="A32" s="10">
         <v>5331</v>
       </c>
-      <c r="B32" s="10">
-        <v>2</v>
+      <c r="B32" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="72" t="s">
         <v>208</v>
       </c>
       <c r="E32" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="F32" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G32" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="33">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="45.75">
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="33"/>
+    </row>
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" s="10">
         <v>5331</v>
       </c>
       <c r="B33" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="67" t="s">
-        <v>225</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D33" s="73"/>
       <c r="E33" s="34" t="s">
         <v>167</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="H33" s="34" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="I33" s="33">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="61">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15">
       <c r="A34" s="10">
-        <v>5331</v>
+        <v>5340</v>
       </c>
       <c r="B34" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D34" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" s="72" t="s">
         <v>209</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="H34" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I34" s="33">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="61">
+    <row r="35" spans="1:9" ht="15">
       <c r="A35" s="10">
-        <v>5331</v>
+        <v>5340</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" s="72" t="s">
-        <v>210</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D35" s="73"/>
       <c r="E35" s="34" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F35" s="33"/>
       <c r="G35" s="33"/>
       <c r="H35" s="34"/>
       <c r="I35" s="33"/>
     </row>
-    <row r="36" spans="1:9" ht="30.5">
+    <row r="36" spans="1:9" ht="15">
       <c r="A36" s="10">
-        <v>5331</v>
+        <v>5341</v>
       </c>
       <c r="B36" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D36" s="73"/>
+        <v>109</v>
+      </c>
+      <c r="D36" s="75" t="s">
+        <v>210</v>
+      </c>
       <c r="E36" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="I36" s="33">
-        <v>33</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="44.25" customHeight="1">
       <c r="A37" s="10">
-        <v>5340</v>
-      </c>
-      <c r="B37" s="10">
+        <v>5341</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="76"/>
+      <c r="E37" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="33"/>
+    </row>
+    <row r="38" spans="1:9" ht="15">
+      <c r="A38" s="10">
+        <v>5352</v>
+      </c>
+      <c r="B38" s="10">
         <v>1</v>
       </c>
-      <c r="C37" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="D37" s="72" t="s">
+      <c r="C38" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="E37" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="F37" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G37" s="33" t="s">
+      <c r="E38" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="H37" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I37" s="33">
+      <c r="I38" s="33">
         <v>110</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="45.75">
-      <c r="A38" s="10">
-        <v>5340</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="D38" s="73"/>
-      <c r="E38" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="33"/>
     </row>
     <row r="39" spans="1:9" ht="27" customHeight="1">
       <c r="A39" s="10">
-        <v>5341</v>
-      </c>
-      <c r="B39" s="10">
-        <v>1</v>
+        <v>5352</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="75" t="s">
-        <v>212</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D39" s="78"/>
       <c r="E39" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="F39" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G39" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="H39" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I39" s="33">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.25">
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="33"/>
+    </row>
+    <row r="40" spans="1:9" ht="15">
       <c r="A40" s="10">
-        <v>5341</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>164</v>
+        <v>5356</v>
+      </c>
+      <c r="B40" s="10">
+        <v>1</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="76"/>
+        <v>173</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>203</v>
+      </c>
       <c r="E40" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="33"/>
-    </row>
-    <row r="41" spans="1:9" ht="30.5">
+        <v>174</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="H40" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" s="33">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" s="10">
-        <v>5352</v>
+        <v>5363</v>
       </c>
       <c r="B41" s="10">
         <v>1</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41" s="77" t="s">
-        <v>213</v>
+        <v>177</v>
+      </c>
+      <c r="D41" s="72" t="s">
+        <v>212</v>
       </c>
       <c r="E41" s="34" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="I41" s="33">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="30.5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15">
       <c r="A42" s="10">
-        <v>5352</v>
+        <v>5363</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" s="78"/>
+        <v>177</v>
+      </c>
+      <c r="D42" s="73"/>
       <c r="E42" s="34" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
@@ -3551,42 +3537,42 @@
     </row>
     <row r="43" spans="1:9" ht="35.25" customHeight="1">
       <c r="A43" s="10">
-        <v>5356</v>
+        <v>5368</v>
       </c>
       <c r="B43" s="10">
         <v>1</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>205</v>
+        <v>156</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>213</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="H43" s="34" t="s">
-        <v>178</v>
+        <v>105</v>
       </c>
       <c r="I43" s="33">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="30.5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15">
       <c r="A44" s="10">
-        <v>5363</v>
+        <v>5373</v>
       </c>
       <c r="B44" s="10">
         <v>1</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D44" s="72" t="s">
         <v>214</v>
@@ -3595,27 +3581,27 @@
         <v>180</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G44" s="33" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="H44" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I44" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30.5">
+    <row r="45" spans="1:9" ht="15">
       <c r="A45" s="10">
-        <v>5363</v>
+        <v>5373</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D45" s="73"/>
       <c r="E45" s="34" t="s">
@@ -3626,123 +3612,123 @@
       <c r="H45" s="34"/>
       <c r="I45" s="33"/>
     </row>
-    <row r="46" spans="1:9" ht="30.5">
+    <row r="46" spans="1:9" ht="15">
       <c r="A46" s="10">
-        <v>5368</v>
+        <v>5375</v>
       </c>
       <c r="B46" s="10">
         <v>1</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D46" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D46" s="75" t="s">
         <v>215</v>
       </c>
       <c r="E46" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="H46" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I46" s="33">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15">
+      <c r="A47" s="10">
+        <v>5375</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="F46" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G46" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="H46" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="I46" s="33">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="30.5">
-      <c r="A47" s="10">
-        <v>5373</v>
-      </c>
-      <c r="B47" s="10">
-        <v>1</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="D47" s="72" t="s">
-        <v>216</v>
-      </c>
+      <c r="D47" s="76"/>
       <c r="E47" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="F47" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G47" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="H47" s="34" t="s">
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="33"/>
+    </row>
+    <row r="48" spans="1:9" ht="15">
+      <c r="A48" s="10">
+        <v>5379</v>
+      </c>
+      <c r="B48" s="10">
+        <v>1</v>
+      </c>
+      <c r="C48" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I47" s="33">
+      <c r="D48" s="61" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="F48" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="H48" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I48" s="33">
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30.5">
-      <c r="A48" s="10">
-        <v>5373</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="D48" s="73"/>
-      <c r="E48" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="33"/>
-    </row>
-    <row r="49" spans="1:10" ht="45.75">
+    <row r="49" spans="1:10" ht="15">
       <c r="A49" s="10">
-        <v>5375</v>
+        <v>5381</v>
       </c>
       <c r="B49" s="10">
         <v>1</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="D49" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="72" t="s">
         <v>217</v>
       </c>
       <c r="E49" s="34" t="s">
         <v>184</v>
       </c>
       <c r="F49" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G49" s="33" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I49" s="33">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="45.75">
+    <row r="50" spans="1:10" ht="15">
       <c r="A50" s="10">
-        <v>5375</v>
+        <v>5381</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="D50" s="76"/>
+        <v>112</v>
+      </c>
+      <c r="D50" s="73"/>
       <c r="E50" s="34" t="s">
         <v>184</v>
       </c>
@@ -3751,246 +3737,168 @@
       <c r="H50" s="34"/>
       <c r="I50" s="33"/>
     </row>
-    <row r="51" spans="1:10" ht="30.5">
+    <row r="51" spans="1:10" ht="15">
       <c r="A51" s="10">
-        <v>5379</v>
+        <v>5383</v>
       </c>
       <c r="B51" s="10">
         <v>1</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D51" s="61" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="10" t="s">
         <v>218</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>185</v>
+        <v>128</v>
       </c>
       <c r="F51" s="33" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="I51" s="33">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="30.5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15">
       <c r="A52" s="10">
-        <v>5381</v>
+        <v>5384</v>
       </c>
       <c r="B52" s="10">
         <v>1</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D52" s="72" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="26" t="s">
         <v>219</v>
       </c>
       <c r="E52" s="34" t="s">
         <v>186</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="H52" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I52" s="33">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.25">
+    <row r="53" spans="1:10" ht="15">
       <c r="A53" s="10">
-        <v>5381</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>164</v>
+        <v>5388</v>
+      </c>
+      <c r="B53" s="10">
+        <v>1</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D53" s="73"/>
+        <v>95</v>
+      </c>
+      <c r="D53" s="72" t="s">
+        <v>220</v>
+      </c>
       <c r="E53" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="33"/>
+        <v>187</v>
+      </c>
+      <c r="F53" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="H53" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I53" s="33">
+        <v>110</v>
+      </c>
     </row>
     <row r="54" spans="1:10" ht="26.25" customHeight="1">
       <c r="A54" s="10">
-        <v>5383</v>
-      </c>
-      <c r="B54" s="10">
-        <v>1</v>
+        <v>5388</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>220</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D54" s="73"/>
       <c r="E54" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="F54" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G54" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="H54" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I54" s="33">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="45.75">
-      <c r="A55" s="10">
-        <v>5384</v>
-      </c>
-      <c r="B55" s="10">
-        <v>1</v>
-      </c>
-      <c r="C55" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="D55" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="E55" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="F55" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G55" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="H55" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I55" s="33">
-        <v>110</v>
-      </c>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="33"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10" ht="60" customHeight="1">
-      <c r="A56" s="10">
-        <v>5388</v>
-      </c>
-      <c r="B56" s="10">
-        <v>1</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="E56" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="F56" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G56" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="H56" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I56" s="33">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.25">
-      <c r="A57" s="10">
-        <v>5388</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="73"/>
-      <c r="E57" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="33"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="40"/>
+      <c r="J57" s="74"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="1"/>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="41"/>
-      <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="74"/>
-    </row>
-    <row r="61" spans="1:10" ht="20.25" customHeight="1">
-      <c r="J61" s="74"/>
-    </row>
+      <c r="J58" s="74"/>
+    </row>
+    <row r="59" spans="1:10"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="14">
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A26:J27"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="J57:J58"/>
     <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D52:D53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>